<commit_message>
Actualizo Hoja Precio Vivienda Idealista. Hago referencia a 2016
</commit_message>
<xml_diff>
--- a/Histórico Precios Alquiler Cádiz (m2) - Fuente Idealista.xlsx
+++ b/Histórico Precios Alquiler Cádiz (m2) - Fuente Idealista.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5eba5648f751a5dd/Documentos/GitHub/openrta-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{3B8E5AAB-590D-432F-ABEF-7D23B72C2F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97554161-E427-43B0-805F-53EE33E459C2}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{3B8E5AAB-590D-432F-ABEF-7D23B72C2F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38046A70-0374-4AE6-AA2B-3077A2361703}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CB6EE892-56B0-4762-9E28-271310B87A4A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB6EE892-56B0-4762-9E28-271310B87A4A}"/>
   </bookViews>
   <sheets>
-    <sheet name="% Incremento Alquiler" sheetId="3" r:id="rId1"/>
+    <sheet name="% Precio Alquiler base 2016" sheetId="3" r:id="rId1"/>
     <sheet name="Precio Alquiler" sheetId="6" r:id="rId2"/>
     <sheet name="Histórico Precio Alquiler Cádiz" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -22,8 +22,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
-    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Mes</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Precio 80m2</t>
-  </si>
-  <si>
-    <t>2015</t>
   </si>
   <si>
     <t>Promedio de Precio 80m2</t>
@@ -189,7 +186,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Histórico Precios Alquiler Cádiz (m2) - Fuente Idealista.xlsx]% Incremento Alquiler!TablaDinámica1</c:name>
+    <c:name>[Histórico Precios Alquiler Cádiz (m2) - Fuente Idealista.xlsx]% Precio Alquiler base 2016!TablaDinámica1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -349,7 +346,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'% Incremento Alquiler'!$B$1</c:f>
+              <c:f>'% Precio Alquiler base 2016'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -370,37 +367,34 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'% Incremento Alquiler'!$A$2:$A$12</c:f>
+              <c:f>'% Precio Alquiler base 2016'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2015</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016</c:v>
+                  <c:v>2017</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017</c:v>
+                  <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018</c:v>
+                  <c:v>2019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021</c:v>
+                  <c:v>2022</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022</c:v>
+                  <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>2024</c:v>
                 </c:pt>
               </c:strCache>
@@ -408,36 +402,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'% Incremento Alquiler'!$B$2:$B$12</c:f>
+              <c:f>'% Precio Alquiler base 2016'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="1">
-                  <c:v>1.8599562363238502E-2</c:v>
+                  <c:v>3.3297529538130866E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.2516411378555609E-2</c:v>
+                  <c:v>7.9484425349086951E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9562363238511961E-2</c:v>
+                  <c:v>0.13211600429645534</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15317286652078765</c:v>
+                  <c:v>0.19441460794844259</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2166301969365427</c:v>
+                  <c:v>0.24060150375939843</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26367614879649881</c:v>
+                  <c:v>0.30397422126745433</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32822757111597373</c:v>
+                  <c:v>0.37916219119226646</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40481400437636766</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.4551422319474836</c:v>
+                  <c:v>0.42857142857142855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,37 +797,34 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Precio Alquiler'!$A$2:$A$12</c:f>
+              <c:f>'Precio Alquiler'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2015</c:v>
+                  <c:v>2016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016</c:v>
+                  <c:v>2017</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017</c:v>
+                  <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018</c:v>
+                  <c:v>2019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021</c:v>
+                  <c:v>2022</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022</c:v>
+                  <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>2024</c:v>
                 </c:pt>
               </c:strCache>
@@ -844,38 +832,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Precio Alquiler'!$B$2:$B$12</c:f>
+              <c:f>'Precio Alquiler'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>609.33333333333337</c:v>
+                  <c:v>620.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>620.66666666666663</c:v>
+                  <c:v>641.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>641.33333333333337</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>670</c:v>
+                  <c:v>702.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>702.66666666666663</c:v>
+                  <c:v>741.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>741.33333333333337</c:v>
+                  <c:v>770</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>770</c:v>
+                  <c:v>809.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>809.33333333333337</c:v>
+                  <c:v>856</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>856</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>886.66666666666663</c:v>
                 </c:pt>
               </c:numCache>
@@ -2197,16 +2182,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>967740</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>182879</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2273,6 +2258,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4204,8 +4193,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68CAA6D7-13C8-4716-A94D-7657BC76ACB9}" name="TablaDinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Fecha">
-  <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68CAA6D7-13C8-4716-A94D-7657BC76ACB9}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Fecha">
+  <location ref="A1:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
       <items count="160">
@@ -4409,7 +4398,7 @@
         <item h="1" sd="0" x="2"/>
         <item h="1" sd="0" x="3"/>
         <item h="1" sd="0" x="4"/>
-        <item sd="0" x="5"/>
+        <item h="1" sd="0" x="5"/>
         <item sd="0" x="6"/>
         <item sd="0" x="7"/>
         <item sd="0" x="8"/>
@@ -4430,10 +4419,7 @@
     <field x="2"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="5"/>
-    </i>
+  <rowItems count="10">
     <i>
       <x v="6"/>
     </i>
@@ -4469,7 +4455,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Promedio de Precio m2" fld="1" subtotal="average" showDataAs="percentDiff" baseField="4" baseItem="5" numFmtId="10"/>
+    <dataField name="Promedio de Precio m2" fld="1" subtotal="average" showDataAs="percentDiff" baseField="4" baseItem="6" numFmtId="10"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="0" series="1">
@@ -4495,8 +4481,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85C3043D-8082-40E1-B345-A533D0299637}" name="TablaDinámica1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Año">
-  <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85C3043D-8082-40E1-B345-A533D0299637}" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Año">
+  <location ref="A1:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
       <items count="161">
@@ -4702,7 +4688,7 @@
         <item h="1" sd="0" x="2"/>
         <item h="1" sd="0" x="3"/>
         <item h="1" sd="0" x="4"/>
-        <item sd="0" x="5"/>
+        <item h="1" sd="0" x="5"/>
         <item sd="0" x="6"/>
         <item sd="0" x="7"/>
         <item sd="0" x="8"/>
@@ -4723,10 +4709,7 @@
     <field x="3"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="5"/>
-    </i>
+  <rowItems count="10">
     <i>
       <x v="6"/>
     </i>
@@ -5130,10 +5113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7704415F-1FB2-45C3-954B-CB6FA93EF4D1}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5153,87 +5136,79 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>1.8599562363238502E-2</v>
+        <v>3.3297529538130866E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4">
-        <v>5.2516411378555609E-2</v>
+        <v>7.9484425349086951E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4">
-        <v>9.9562363238511961E-2</v>
+        <v>0.13211600429645534</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4">
-        <v>0.15317286652078765</v>
+        <v>0.19441460794844259</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4">
-        <v>0.2166301969365427</v>
+        <v>0.24060150375939843</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4">
-        <v>0.26367614879649881</v>
+        <v>0.30397422126745433</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4">
-        <v>0.32822757111597373</v>
+        <v>0.37916219119226646</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="4">
-        <v>0.40481400437636766</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.4551422319474836</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5243,9 +5218,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8071BAAF-B833-4F1E-9762-B122DA0B57DA}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -5257,98 +5232,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5">
-        <v>609.33333333333337</v>
+        <v>620.66666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5">
-        <v>620.66666666666663</v>
+        <v>641.33333333333337</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
-        <v>641.33333333333337</v>
+        <v>670</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5">
-        <v>670</v>
+        <v>702.66666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
-        <v>702.66666666666663</v>
+        <v>741.33333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5">
-        <v>741.33333333333337</v>
+        <v>770</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5">
-        <v>770</v>
+        <v>809.33333333333337</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="5">
-        <v>809.33333333333337</v>
+        <v>856</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="5">
-        <v>856</v>
+        <v>886.66666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B11" s="5">
-        <v>886.66666666666663</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="5">
-        <v>722.52631578947364</v>
+        <v>735.84313725490199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>